<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@102f8a974cafadb008518f5a67babdf8d88eabae 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-6694184095798346213" xfId="1" hidden="0"/>
-    <cellStyle name="-5292336233671759821" xfId="2" hidden="0"/>
+    <cellStyle name="5897753757051097329" xfId="1" hidden="0"/>
+    <cellStyle name="-7817928977278746789" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -480,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ1"/>
+  <dimension ref="A1:BL1"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,6 +550,8 @@
     <col width="20" customWidth="1" min="60" max="60"/>
     <col width="20" customWidth="1" min="61" max="61"/>
     <col width="20" customWidth="1" min="62" max="62"/>
+    <col width="20" customWidth="1" min="63" max="63"/>
+    <col width="20" customWidth="1" min="64" max="64"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -645,220 +647,230 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>INDIVIDUAL_REF_ID</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>INDIVIDUAL_REF_DB</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>CELL_INPUT[TOTAL_ALIVE CELLS]</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>TISSUE_PREP_METHOD</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>NA_PREP_METHOD</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>QUBIT_NA_CONC[ng/ul]</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>NOTES</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>LIB_PREP_KIT</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>LIBRARY_TYPE</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>NA_INPUT_QUANTITY [ng]</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>NA_INPUT_QUANTITY [ul]</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>PCR_CYCLES_FIRST_AMP</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>PCR_CYCLES_SECOND_AMP</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>LIBRARY_CONC[ng/ul]</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>AVERAGE_FRAGMENT_SIZE</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>LIBRARY_MOLARITY[nmol]</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>BARCODETYPE</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_WELL_I5</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_SEQ_I5</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_WELL_I7</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_SEQ_I7</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>DNA_FRAGMENTATION_METHOD</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>IMAGING_DATASET</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>IMAGING_DATASET_ID</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>SEQUENCER</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>MULTIPLEX</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>MULTIPLEX_NAME</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>LANES_TOTAL</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>ILSE_NO</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>DATE_OF_SUBM</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>EXPER_LOCATION</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>PLATE</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>WELL_COLUMN</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>WELL_ROW</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>WELL</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY_TARGET</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY_LOT</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>AMPURE_LOT</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>DYNABEADS_LOT</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>QUIBIT_LOT</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>CLARIOSTAR_LOT</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>NA_PREP_LOT</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>ENZYM_FRAG_LOT</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>LIBRARYPREP_KIT_LOT</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>INDEXPRIMER_LOT</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>CAPTURE_PROBES_LOT</t>
         </is>
@@ -875,7 +887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ6"/>
+  <dimension ref="A1:BL6"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -946,6 +958,8 @@
     <col width="20" customWidth="1" min="60" max="60"/>
     <col width="20" customWidth="1" min="61" max="61"/>
     <col width="20" customWidth="1" min="62" max="62"/>
+    <col width="20" customWidth="1" min="63" max="63"/>
+    <col width="20" customWidth="1" min="64" max="64"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -1041,220 +1055,230 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>INDIVIDUAL_REF_ID</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>INDIVIDUAL_REF_DB</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>CELL_INPUT[TOTAL_ALIVE CELLS]</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>TISSUE_PREP_METHOD</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>NA_PREP_METHOD</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>QUBIT_NA_CONC[ng/ul]</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>NOTES</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>LIB_PREP_KIT</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>LIBRARY_TYPE</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>NA_INPUT_QUANTITY [ng]</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>NA_INPUT_QUANTITY [ul]</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>PCR_CYCLES_FIRST_AMP</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>PCR_CYCLES_SECOND_AMP</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>LIBRARY_CONC[ng/ul]</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>AVERAGE_FRAGMENT_SIZE</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>LIBRARY_MOLARITY[nmol]</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>BARCODETYPE</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_WELL_I5</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_SEQ_I5</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_WELL_I7</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_SEQ_I7</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>DNA_FRAGMENTATION_METHOD</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>IMAGING_DATASET</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>IMAGING_DATASET_ID</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>SEQUENCER</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>MULTIPLEX</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>MULTIPLEX_NAME</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>LANES_TOTAL</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>ILSE_NO</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>DATE_OF_SUBM</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>EXPER_LOCATION</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>PLATE</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>WELL_COLUMN</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>WELL_ROW</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>WELL</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY_TARGET</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY_LOT</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>AMPURE_LOT</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>DYNABEADS_LOT</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>QUIBIT_LOT</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>CLARIOSTAR_LOT</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>NA_PREP_LOT</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>ENZYM_FRAG_LOT</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>LIBRARYPREP_KIT_LOT</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>INDEXPRIMER_LOT</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>CAPTURE_PROBES_LOT</t>
         </is>
@@ -1353,220 +1377,230 @@
       </c>
       <c r="S2" s="2" t="inlineStr">
         <is>
+          <t>ID/Label of the individual as referenced to in external database</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="inlineStr">
+        <is>
+          <t>Label of the external mouse database e.g. MoVi / CRUK-CI</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
           <t>Number of cell (if available) [TOTAL_ALIVE CELLS]</t>
         </is>
       </c>
-      <c r="T2" s="2" t="inlineStr">
+      <c r="V2" s="2" t="inlineStr">
         <is>
           <t>Brief description to method of tissue preparation</t>
         </is>
       </c>
-      <c r="U2" s="2" t="inlineStr">
+      <c r="W2" s="2" t="inlineStr">
         <is>
           <t>Method (probably a kit) used to extract nucleic acid (NA)</t>
         </is>
       </c>
-      <c r="V2" s="2" t="inlineStr">
+      <c r="X2" s="2" t="inlineStr">
         <is>
           <t>DNA/RNA concentration measured by Qubit [ng/ul]</t>
         </is>
       </c>
-      <c r="W2" s="2" t="inlineStr">
+      <c r="Y2" s="2" t="inlineStr">
         <is>
           <t>Any additional notes, comments for the submission</t>
         </is>
       </c>
-      <c r="X2" s="2" t="inlineStr">
+      <c r="Z2" s="2" t="inlineStr">
         <is>
           <t>If using a new Kit, check first with ODCF because they need to register it to their database. Use their descriptor.</t>
         </is>
       </c>
-      <c r="Y2" s="2" t="inlineStr">
+      <c r="AA2" s="2" t="inlineStr">
         <is>
           <t>Type of library and how it was generated.</t>
         </is>
       </c>
-      <c r="Z2" s="2" t="inlineStr">
+      <c r="AB2" s="2" t="inlineStr">
         <is>
           <t>Mass of input RNA/DNA</t>
         </is>
       </c>
-      <c r="AA2" s="2" t="inlineStr">
+      <c r="AC2" s="2" t="inlineStr">
         <is>
           <t>Volume of input RNA/DNA</t>
         </is>
       </c>
-      <c r="AB2" s="2" t="inlineStr">
+      <c r="AD2" s="2" t="inlineStr">
         <is>
           <t>Number of PCR cycles in first amplication</t>
         </is>
       </c>
-      <c r="AC2" s="2" t="inlineStr">
+      <c r="AE2" s="2" t="inlineStr">
         <is>
           <t>Number of PCR cycles in second amplication</t>
         </is>
       </c>
-      <c r="AD2" s="2" t="inlineStr">
+      <c r="AF2" s="2" t="inlineStr">
         <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="AE2" s="2" t="inlineStr">
+      <c r="AG2" s="2" t="inlineStr">
         <is>
           <t>Average fragment length (basepairs=</t>
         </is>
       </c>
-      <c r="AF2" s="2" t="inlineStr">
+      <c r="AH2" s="2" t="inlineStr">
         <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="AG2" s="2" t="inlineStr">
+      <c r="AI2" s="2" t="inlineStr">
         <is>
           <t>Description of barcode used</t>
         </is>
       </c>
-      <c r="AH2" s="2" t="inlineStr">
+      <c r="AJ2" s="2" t="inlineStr">
         <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="AI2" s="2" t="inlineStr">
+      <c r="AK2" s="2" t="inlineStr">
         <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="AJ2" s="2" t="inlineStr">
+      <c r="AL2" s="2" t="inlineStr">
         <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="AK2" s="2" t="inlineStr">
+      <c r="AM2" s="2" t="inlineStr">
         <is>
           <t>Sequence of the I7 barcode (for 10x-singcell this can be a comma-separated list of 4 indeces)</t>
         </is>
       </c>
-      <c r="AL2" s="2" t="inlineStr">
+      <c r="AN2" s="2" t="inlineStr">
         <is>
           <t>Method used to fragment DNA</t>
         </is>
       </c>
-      <c r="AM2" s="2" t="inlineStr">
+      <c r="AO2" s="2" t="inlineStr">
         <is>
           <t>Imaging dataset for Spatial Transcriptomics</t>
         </is>
       </c>
-      <c r="AN2" s="2" t="inlineStr">
+      <c r="AP2" s="2" t="inlineStr">
         <is>
           <t>Free-txt description of sequencing platforms, read-length and run-type (for your information and submission to the sequencing center)</t>
         </is>
       </c>
-      <c r="AO2" s="2" t="inlineStr">
+      <c r="AQ2" s="2" t="inlineStr">
         <is>
           <t>Number of samples in Multiplex</t>
         </is>
       </c>
-      <c r="AP2" s="2" t="inlineStr">
+      <c r="AR2" s="2" t="inlineStr">
         <is>
           <t>Your initials followed by the date of submission format(ABYYYYMMDD)</t>
         </is>
       </c>
-      <c r="AQ2" s="2" t="inlineStr">
+      <c r="AS2" s="2" t="inlineStr">
         <is>
           <t>Number of lanes sequenced</t>
         </is>
       </c>
-      <c r="AR2" s="2" t="inlineStr">
+      <c r="AT2" s="2" t="inlineStr">
         <is>
           <t>ILSE number as provided by GPCF/ILSe</t>
         </is>
       </c>
-      <c r="AS2" s="2" t="inlineStr">
+      <c r="AU2" s="2" t="inlineStr">
         <is>
           <t>When was the sample submitted for sequencing? (format YYYY-MM-DD)</t>
         </is>
       </c>
-      <c r="AT2" s="2" t="inlineStr">
+      <c r="AV2" s="2" t="inlineStr">
         <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="AU2" s="2" t="inlineStr">
+      <c r="AW2" s="2" t="inlineStr">
         <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="AV2" s="2" t="inlineStr">
+      <c r="AX2" s="2" t="inlineStr">
         <is>
           <t>Column in the plate</t>
         </is>
       </c>
-      <c r="AW2" s="2" t="inlineStr">
+      <c r="AY2" s="2" t="inlineStr">
         <is>
           <t>Row in the plate</t>
         </is>
       </c>
-      <c r="AX2" s="2" t="inlineStr">
+      <c r="AZ2" s="2" t="inlineStr">
         <is>
           <t>REQUIRED FOR SMARTSEQ2, combination of column and row</t>
         </is>
       </c>
-      <c r="AY2" s="2" t="inlineStr">
+      <c r="BA2" s="2" t="inlineStr">
         <is>
           <t>Antibody target protein</t>
         </is>
       </c>
-      <c r="AZ2" s="2" t="inlineStr">
+      <c r="BB2" s="2" t="inlineStr">
         <is>
           <t>Antibody name, manufacturer etc.</t>
         </is>
       </c>
-      <c r="BA2" s="2" t="inlineStr">
+      <c r="BC2" s="2" t="inlineStr">
         <is>
           <t>LOT number of the antibody</t>
         </is>
       </c>
-      <c r="BB2" s="2" t="inlineStr">
+      <c r="BD2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BC2" s="2" t="inlineStr">
+      <c r="BE2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BD2" s="2" t="inlineStr">
+      <c r="BF2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BE2" s="2" t="inlineStr">
+      <c r="BG2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BF2" s="2" t="inlineStr">
+      <c r="BH2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BG2" s="2" t="inlineStr">
+      <c r="BI2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BH2" s="2" t="inlineStr">
+      <c r="BJ2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BI2" s="2" t="inlineStr">
+      <c r="BK2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
       </c>
-      <c r="BJ2" s="2" t="inlineStr">
+      <c r="BL2" s="2" t="inlineStr">
         <is>
           <t>LOT number as provided by manufacturer</t>
         </is>
@@ -1659,129 +1693,137 @@
           <t>['acetone 25w_DMBA/TPA 10w_DMBA/TPA DMBA/TPA_or_TPA TPA UV']</t>
         </is>
       </c>
-      <c r="S3" s="2" t="inlineStr"/>
+      <c r="S3" s="2" t="inlineStr">
+        <is>
+          <t>[12345]</t>
+        </is>
+      </c>
       <c r="T3" s="2" t="inlineStr">
         <is>
+          <t>['MoVi, CRUK-CI']</t>
+        </is>
+      </c>
+      <c r="U3" s="2" t="inlineStr"/>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
           <t>['liver_ex Single cell MB RNA/DNATissueLyzerII Single cell C. Ernst 1. Enzymes 2. Trypsin 1. Trypsin 2. Enzymes skinbiopsy']</t>
         </is>
       </c>
-      <c r="U3" s="2" t="inlineStr">
+      <c r="W3" s="2" t="inlineStr">
         <is>
           <t>['Modified Qiagen DNeasy blood&amp;tissue Qiagen Dneasy blood&amp;tissue Qiagen RNeasy micro']</t>
         </is>
       </c>
-      <c r="V3" s="2" t="inlineStr"/>
-      <c r="W3" s="2" t="inlineStr"/>
-      <c r="X3" s="2" t="inlineStr">
+      <c r="X3" s="2" t="inlineStr"/>
+      <c r="Y3" s="2" t="inlineStr"/>
+      <c r="Z3" s="2" t="inlineStr">
         <is>
           <t>['scRNA_10x_v3', 'WGS_NEBNext_ULTRA_II', 'Agilent SureSelect Pre-capture', 'Agilent SureSelect XT Low input Mouse AllExon', 'Agilent SureSelect Post-capture', 'NEBNext RNA Low Input - E6420']</t>
         </is>
       </c>
-      <c r="Y3" s="2" t="inlineStr">
+      <c r="AA3" s="2" t="inlineStr">
         <is>
           <t>['WES_SureSelectXTHS WGS RNA_NEBNext_Low_Input scRNA_10x_v3 RNA_SMARTSeq_v4_Ultra_Low_Input scATAC scRNA_10x_nextgem']</t>
         </is>
       </c>
-      <c r="Z3" s="2" t="inlineStr"/>
-      <c r="AA3" s="2" t="inlineStr"/>
       <c r="AB3" s="2" t="inlineStr"/>
       <c r="AC3" s="2" t="inlineStr"/>
-      <c r="AD3" s="2" t="n">
+      <c r="AD3" s="2" t="inlineStr"/>
+      <c r="AE3" s="2" t="inlineStr"/>
+      <c r="AF3" s="2" t="n">
         <v>14.4</v>
       </c>
-      <c r="AE3" s="2" t="n">
+      <c r="AG3" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="AF3" s="2" t="n">
+      <c r="AH3" s="2" t="n">
         <v>46.94</v>
       </c>
-      <c r="AG3" s="2" t="inlineStr">
+      <c r="AI3" s="2" t="inlineStr">
         <is>
           <t>['SureSelect 16 Rxn 10X Chromium v3 NEB 96 oligos SureSelect 96 rxn']</t>
         </is>
       </c>
-      <c r="AH3" s="2" t="inlineStr">
+      <c r="AJ3" s="2" t="inlineStr">
         <is>
           <t>A7, N701, SI-GA-A6</t>
         </is>
       </c>
-      <c r="AI3" s="2" t="inlineStr">
+      <c r="AK3" s="2" t="inlineStr">
         <is>
           <t>TTACCGAC, TATCCTCT</t>
         </is>
       </c>
-      <c r="AJ3" s="2" t="inlineStr">
+      <c r="AL3" s="2" t="inlineStr">
         <is>
           <t>A7, S503</t>
         </is>
       </c>
-      <c r="AK3" s="2" t="inlineStr">
+      <c r="AM3" s="2" t="inlineStr">
         <is>
           <t>TTACCGAC, GCGAGTAA</t>
         </is>
       </c>
-      <c r="AL3" s="2" t="inlineStr">
+      <c r="AN3" s="2" t="inlineStr">
         <is>
           <t>['enzymatic sonicator']</t>
         </is>
       </c>
-      <c r="AM3" s="2" t="inlineStr">
+      <c r="AO3" s="2" t="inlineStr">
         <is>
           <t>['DOIMG-00001']</t>
         </is>
       </c>
-      <c r="AN3" s="2" t="inlineStr">
+      <c r="AP3" s="2" t="inlineStr">
         <is>
           <t>NextSeq 550 Paired-End 75bp Mid-Output</t>
         </is>
       </c>
-      <c r="AO3" s="2" t="n">
+      <c r="AQ3" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="AP3" s="2" t="inlineStr">
+      <c r="AR3" s="2" t="inlineStr">
         <is>
           <t>MB20190923</t>
         </is>
       </c>
-      <c r="AQ3" s="2" t="n">
+      <c r="AS3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AR3" s="2" t="n">
+      <c r="AT3" s="2" t="n">
         <v>12345</v>
       </c>
-      <c r="AS3" s="2" t="n">
+      <c r="AU3" s="2" t="n">
         <v>44135</v>
       </c>
-      <c r="AT3" s="2" t="inlineStr">
+      <c r="AV3" s="2" t="inlineStr">
         <is>
           <t>['MB_folder', 'AT1_15_A1', 'AT1_45_A1']</t>
         </is>
       </c>
-      <c r="AU3" s="2" t="inlineStr">
+      <c r="AW3" s="2" t="inlineStr">
         <is>
           <t>['T1 plate 1', 20200130]</t>
         </is>
       </c>
-      <c r="AV3" s="2" t="n">
+      <c r="AX3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AW3" s="2" t="inlineStr">
+      <c r="AY3" s="2" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="AX3" s="2" t="inlineStr">
+      <c r="AZ3" s="2" t="inlineStr">
         <is>
           <t>1A</t>
         </is>
       </c>
-      <c r="AY3" s="2" t="inlineStr">
+      <c r="BA3" s="2" t="inlineStr">
         <is>
           <t>HNF4A, CEBPA</t>
         </is>
       </c>
-      <c r="AZ3" s="2" t="inlineStr"/>
-      <c r="BA3" s="2" t="inlineStr"/>
       <c r="BB3" s="2" t="inlineStr"/>
       <c r="BC3" s="2" t="inlineStr"/>
       <c r="BD3" s="2" t="inlineStr"/>
@@ -1791,6 +1833,8 @@
       <c r="BH3" s="2" t="inlineStr"/>
       <c r="BI3" s="2" t="inlineStr"/>
       <c r="BJ3" s="2" t="inlineStr"/>
+      <c r="BK3" s="2" t="inlineStr"/>
+      <c r="BL3" s="2" t="inlineStr"/>
     </row>
     <row r="4" ht="25" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -1906,19 +1950,19 @@
       </c>
       <c r="X4" s="2" t="inlineStr">
         <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="Y4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="Z4" s="2" t="inlineStr">
+        <is>
           <t>Odomlab, GUIDE, OTP</t>
         </is>
       </c>
-      <c r="Y4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
-      <c r="Z4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
       <c r="AA4" s="2" t="inlineStr">
         <is>
           <t>Odomlab</t>
@@ -1986,19 +2030,19 @@
       </c>
       <c r="AN4" s="2" t="inlineStr">
         <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AO4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AP4" s="2" t="inlineStr">
+        <is>
           <t>None</t>
         </is>
       </c>
-      <c r="AO4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
-      <c r="AP4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
       <c r="AQ4" s="2" t="inlineStr">
         <is>
           <t>Odomlab</t>
@@ -2006,19 +2050,19 @@
       </c>
       <c r="AR4" s="2" t="inlineStr">
         <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AS4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AT4" s="2" t="inlineStr">
+        <is>
           <t>GUIDE, Odomlab</t>
         </is>
       </c>
-      <c r="AS4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
-      <c r="AT4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
       <c r="AU4" s="2" t="inlineStr">
         <is>
           <t>Odomlab</t>
@@ -2059,17 +2103,17 @@
           <t>Odomlab</t>
         </is>
       </c>
-      <c r="BC4" s="2" t="inlineStr"/>
+      <c r="BC4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
       <c r="BD4" s="2" t="inlineStr">
         <is>
           <t>Odomlab</t>
         </is>
       </c>
-      <c r="BE4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
+      <c r="BE4" s="2" t="inlineStr"/>
       <c r="BF4" s="2" t="inlineStr">
         <is>
           <t>Odomlab</t>
@@ -2091,6 +2135,16 @@
         </is>
       </c>
       <c r="BJ4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BK4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BL4" s="2" t="inlineStr">
         <is>
           <t>Odomlab</t>
         </is>
@@ -2189,220 +2243,230 @@
       </c>
       <c r="S5" s="2" t="inlineStr">
         <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="U5" s="2" t="inlineStr">
+        <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="T5" s="2" t="inlineStr">
+      <c r="V5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="U5" s="2" t="inlineStr">
+      <c r="W5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="V5" s="2" t="inlineStr">
+      <c r="X5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="W5" s="2" t="inlineStr">
+      <c r="Y5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="X5" s="2" t="inlineStr">
+      <c r="Z5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="Y5" s="2" t="inlineStr">
+      <c r="AA5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="Z5" s="2" t="inlineStr">
+      <c r="AB5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AA5" s="2" t="inlineStr">
+      <c r="AC5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AB5" s="2" t="inlineStr">
+      <c r="AD5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AC5" s="2" t="inlineStr">
+      <c r="AE5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AD5" s="2" t="inlineStr">
+      <c r="AF5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AE5" s="2" t="inlineStr">
+      <c r="AG5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AF5" s="2" t="inlineStr">
+      <c r="AH5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AG5" s="2" t="inlineStr">
+      <c r="AI5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AH5" s="2" t="inlineStr">
+      <c r="AJ5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AI5" s="2" t="inlineStr">
+      <c r="AK5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AJ5" s="2" t="inlineStr">
+      <c r="AL5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AK5" s="2" t="inlineStr">
+      <c r="AM5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AL5" s="2" t="inlineStr">
+      <c r="AN5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AM5" s="2" t="inlineStr">
+      <c r="AO5" s="2" t="inlineStr">
         <is>
           <t>experiment</t>
         </is>
       </c>
-      <c r="AN5" s="2" t="inlineStr">
+      <c r="AP5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AO5" s="2" t="inlineStr">
+      <c r="AQ5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AP5" s="2" t="inlineStr">
+      <c r="AR5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AQ5" s="2" t="inlineStr">
+      <c r="AS5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AR5" s="2" t="inlineStr">
+      <c r="AT5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AS5" s="2" t="inlineStr">
+      <c r="AU5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AT5" s="2" t="inlineStr">
+      <c r="AV5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AU5" s="2" t="inlineStr">
+      <c r="AW5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AV5" s="2" t="inlineStr">
+      <c r="AX5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AW5" s="2" t="inlineStr">
+      <c r="AY5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AX5" s="2" t="inlineStr">
+      <c r="AZ5" s="2" t="inlineStr">
         <is>
           <t>sequencing</t>
         </is>
       </c>
-      <c r="AY5" s="2" t="inlineStr">
+      <c r="BA5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="AZ5" s="2" t="inlineStr">
+      <c r="BB5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BA5" s="2" t="inlineStr">
+      <c r="BC5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BB5" s="2" t="inlineStr">
+      <c r="BD5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BC5" s="2" t="inlineStr">
+      <c r="BE5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BD5" s="2" t="inlineStr">
+      <c r="BF5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BE5" s="2" t="inlineStr">
+      <c r="BG5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BF5" s="2" t="inlineStr">
+      <c r="BH5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BG5" s="2" t="inlineStr">
+      <c r="BI5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BH5" s="2" t="inlineStr">
+      <c r="BJ5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BI5" s="2" t="inlineStr">
+      <c r="BK5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="BJ5" s="2" t="inlineStr">
+      <c r="BL5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
@@ -2438,97 +2502,97 @@
       <c r="W6" s="2" t="inlineStr"/>
       <c r="X6" s="2" t="inlineStr"/>
       <c r="Y6" s="2" t="inlineStr"/>
-      <c r="Z6" s="2" t="inlineStr">
+      <c r="Z6" s="2" t="inlineStr"/>
+      <c r="AA6" s="2" t="inlineStr"/>
+      <c r="AB6" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AA6" s="2" t="inlineStr">
+      <c r="AC6" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AB6" s="2" t="inlineStr">
+      <c r="AD6" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AC6" s="2" t="inlineStr">
+      <c r="AE6" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AD6" s="2" t="inlineStr">
+      <c r="AF6" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AE6" s="2" t="inlineStr">
+      <c r="AG6" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AF6" s="2" t="inlineStr">
+      <c r="AH6" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AG6" s="2" t="inlineStr"/>
-      <c r="AH6" s="2" t="inlineStr"/>
-      <c r="AI6" s="2" t="inlineStr">
-        <is>
-          <t>[ATGC]*</t>
-        </is>
-      </c>
+      <c r="AI6" s="2" t="inlineStr"/>
       <c r="AJ6" s="2" t="inlineStr"/>
       <c r="AK6" s="2" t="inlineStr">
         <is>
+          <t>[ATGC]*</t>
+        </is>
+      </c>
+      <c r="AL6" s="2" t="inlineStr"/>
+      <c r="AM6" s="2" t="inlineStr">
+        <is>
           <t>[ATGC, ]*</t>
         </is>
       </c>
-      <c r="AL6" s="2" t="inlineStr"/>
-      <c r="AM6" s="2" t="inlineStr"/>
       <c r="AN6" s="2" t="inlineStr"/>
-      <c r="AO6" s="2" t="inlineStr">
+      <c r="AO6" s="2" t="inlineStr"/>
+      <c r="AP6" s="2" t="inlineStr"/>
+      <c r="AQ6" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AP6" s="2" t="inlineStr">
+      <c r="AR6" s="2" t="inlineStr">
         <is>
           <t>[A-Z]{2}[0-9]{4}[0-9]{2}[0-9]{2}</t>
         </is>
       </c>
-      <c r="AQ6" s="2" t="inlineStr">
+      <c r="AS6" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AR6" s="2" t="inlineStr">
+      <c r="AT6" s="2" t="inlineStr">
         <is>
           <t>[0-9]{5,}</t>
         </is>
       </c>
-      <c r="AS6" s="2" t="inlineStr"/>
-      <c r="AT6" s="2" t="inlineStr"/>
       <c r="AU6" s="2" t="inlineStr"/>
-      <c r="AV6" s="2" t="inlineStr">
+      <c r="AV6" s="2" t="inlineStr"/>
+      <c r="AW6" s="2" t="inlineStr"/>
+      <c r="AX6" s="2" t="inlineStr">
         <is>
           <t>[0-9]{1,2}</t>
         </is>
       </c>
-      <c r="AW6" s="2" t="inlineStr">
+      <c r="AY6" s="2" t="inlineStr">
         <is>
           <t>[A-Z]</t>
         </is>
       </c>
-      <c r="AX6" s="2" t="inlineStr">
+      <c r="AZ6" s="2" t="inlineStr">
         <is>
           <t>[0-9]{1,2}[A-Z]</t>
         </is>
       </c>
-      <c r="AY6" s="2" t="inlineStr"/>
-      <c r="AZ6" s="2" t="inlineStr"/>
       <c r="BA6" s="2" t="inlineStr"/>
       <c r="BB6" s="2" t="inlineStr"/>
       <c r="BC6" s="2" t="inlineStr"/>
@@ -2539,6 +2603,8 @@
       <c r="BH6" s="2" t="inlineStr"/>
       <c r="BI6" s="2" t="inlineStr"/>
       <c r="BJ6" s="2" t="inlineStr"/>
+      <c r="BK6" s="2" t="inlineStr"/>
+      <c r="BL6" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@d14bffbbb439d5af4f50ba8554a3eee18e1d14ef 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="5897753757051097329" xfId="1" hidden="0"/>
-    <cellStyle name="-7817928977278746789" xfId="2" hidden="0"/>
+    <cellStyle name="2037184015289833625" xfId="1" hidden="0"/>
+    <cellStyle name="6508422940602682099" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1367,112 +1367,112 @@
       </c>
       <c r="Q2" s="2" t="inlineStr">
         <is>
+          <t>How was the mouse/animal killed?</t>
+        </is>
+      </c>
+      <c r="R2" s="2" t="inlineStr">
+        <is>
+          <t>Any treatment / pertubation applied to the individual/ cell-line.</t>
+        </is>
+      </c>
+      <c r="S2" s="2" t="inlineStr">
+        <is>
+          <t>ID/Label of the individual as referenced to in external database</t>
+        </is>
+      </c>
+      <c r="T2" s="2" t="inlineStr">
+        <is>
+          <t>Label of the external mouse database e.g. MoVi / CRUK-CI</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
+          <t>Number of cell (if available) [TOTAL_ALIVE CELLS]</t>
+        </is>
+      </c>
+      <c r="V2" s="2" t="inlineStr">
+        <is>
+          <t>Brief description to method of tissue preparation</t>
+        </is>
+      </c>
+      <c r="W2" s="2" t="inlineStr">
+        <is>
+          <t>Method (probably a kit) used to extract nucleic acid (NA)</t>
+        </is>
+      </c>
+      <c r="X2" s="2" t="inlineStr">
+        <is>
+          <t>DNA/RNA concentration measured by Qubit [ng/ul]</t>
+        </is>
+      </c>
+      <c r="Y2" s="2" t="inlineStr">
+        <is>
+          <t>Any additional notes, comments for the submission</t>
+        </is>
+      </c>
+      <c r="Z2" s="2" t="inlineStr">
+        <is>
+          <t>If using a new Kit, check first with ODCF because they need to register it to their database. Use their descriptor.</t>
+        </is>
+      </c>
+      <c r="AA2" s="2" t="inlineStr">
+        <is>
+          <t>Type of library and how it was generated.</t>
+        </is>
+      </c>
+      <c r="AB2" s="2" t="inlineStr">
+        <is>
+          <t>Mass of input RNA/DNA</t>
+        </is>
+      </c>
+      <c r="AC2" s="2" t="inlineStr">
+        <is>
+          <t>Volume of input RNA/DNA</t>
+        </is>
+      </c>
+      <c r="AD2" s="2" t="inlineStr">
+        <is>
+          <t>Number of PCR cycles in first amplication</t>
+        </is>
+      </c>
+      <c r="AE2" s="2" t="inlineStr">
+        <is>
+          <t>Number of PCR cycles in second amplication</t>
+        </is>
+      </c>
+      <c r="AF2" s="2" t="inlineStr">
+        <is>
+          <t>Nucleic acid concentration</t>
+        </is>
+      </c>
+      <c r="AG2" s="2" t="inlineStr">
+        <is>
+          <t>Average fragment length (basepairs)</t>
+        </is>
+      </c>
+      <c r="AH2" s="2" t="inlineStr">
+        <is>
+          <t>Library molarity</t>
+        </is>
+      </c>
+      <c r="AI2" s="2" t="inlineStr">
+        <is>
+          <t>Description of barcode used</t>
+        </is>
+      </c>
+      <c r="AJ2" s="2" t="inlineStr">
+        <is>
+          <t>Well position of the barcode</t>
+        </is>
+      </c>
+      <c r="AK2" s="2" t="inlineStr">
+        <is>
           <t>another description</t>
         </is>
       </c>
-      <c r="R2" s="2" t="inlineStr">
-        <is>
-          <t>another description</t>
-        </is>
-      </c>
-      <c r="S2" s="2" t="inlineStr">
-        <is>
-          <t>ID/Label of the individual as referenced to in external database</t>
-        </is>
-      </c>
-      <c r="T2" s="2" t="inlineStr">
-        <is>
-          <t>Label of the external mouse database e.g. MoVi / CRUK-CI</t>
-        </is>
-      </c>
-      <c r="U2" s="2" t="inlineStr">
-        <is>
-          <t>Number of cell (if available) [TOTAL_ALIVE CELLS]</t>
-        </is>
-      </c>
-      <c r="V2" s="2" t="inlineStr">
-        <is>
-          <t>Brief description to method of tissue preparation</t>
-        </is>
-      </c>
-      <c r="W2" s="2" t="inlineStr">
-        <is>
-          <t>Method (probably a kit) used to extract nucleic acid (NA)</t>
-        </is>
-      </c>
-      <c r="X2" s="2" t="inlineStr">
-        <is>
-          <t>DNA/RNA concentration measured by Qubit [ng/ul]</t>
-        </is>
-      </c>
-      <c r="Y2" s="2" t="inlineStr">
-        <is>
-          <t>Any additional notes, comments for the submission</t>
-        </is>
-      </c>
-      <c r="Z2" s="2" t="inlineStr">
-        <is>
-          <t>If using a new Kit, check first with ODCF because they need to register it to their database. Use their descriptor.</t>
-        </is>
-      </c>
-      <c r="AA2" s="2" t="inlineStr">
-        <is>
-          <t>Type of library and how it was generated.</t>
-        </is>
-      </c>
-      <c r="AB2" s="2" t="inlineStr">
-        <is>
-          <t>Mass of input RNA/DNA</t>
-        </is>
-      </c>
-      <c r="AC2" s="2" t="inlineStr">
-        <is>
-          <t>Volume of input RNA/DNA</t>
-        </is>
-      </c>
-      <c r="AD2" s="2" t="inlineStr">
-        <is>
-          <t>Number of PCR cycles in first amplication</t>
-        </is>
-      </c>
-      <c r="AE2" s="2" t="inlineStr">
-        <is>
-          <t>Number of PCR cycles in second amplication</t>
-        </is>
-      </c>
-      <c r="AF2" s="2" t="inlineStr">
-        <is>
-          <t>another description</t>
-        </is>
-      </c>
-      <c r="AG2" s="2" t="inlineStr">
-        <is>
-          <t>Average fragment length (basepairs=</t>
-        </is>
-      </c>
-      <c r="AH2" s="2" t="inlineStr">
-        <is>
-          <t>another description</t>
-        </is>
-      </c>
-      <c r="AI2" s="2" t="inlineStr">
-        <is>
-          <t>Description of barcode used</t>
-        </is>
-      </c>
-      <c r="AJ2" s="2" t="inlineStr">
-        <is>
-          <t>another description</t>
-        </is>
-      </c>
-      <c r="AK2" s="2" t="inlineStr">
-        <is>
-          <t>another description</t>
-        </is>
-      </c>
       <c r="AL2" s="2" t="inlineStr">
         <is>
-          <t>another description</t>
+          <t>Well position of the barcode</t>
         </is>
       </c>
       <c r="AM2" s="2" t="inlineStr">
@@ -1522,12 +1522,12 @@
       </c>
       <c r="AV2" s="2" t="inlineStr">
         <is>
-          <t>another description</t>
+          <t>Location of the library/experiement description</t>
         </is>
       </c>
       <c r="AW2" s="2" t="inlineStr">
         <is>
-          <t>another description</t>
+          <t>Plate label used</t>
         </is>
       </c>
       <c r="AX2" s="2" t="inlineStr">
@@ -2491,8 +2491,16 @@
       <c r="L6" s="2" t="inlineStr"/>
       <c r="M6" s="2" t="inlineStr"/>
       <c r="N6" s="2" t="inlineStr"/>
-      <c r="O6" s="2" t="inlineStr"/>
-      <c r="P6" s="2" t="inlineStr"/>
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>[0-9]{4}-[0-9]{2}-[0-9]{2}</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="inlineStr">
+        <is>
+          <t>[0-9]{4}-[0-9]{2}-[0-9]{2}</t>
+        </is>
+      </c>
       <c r="Q6" s="2" t="inlineStr"/>
       <c r="R6" s="2" t="inlineStr"/>
       <c r="S6" s="2" t="inlineStr"/>
@@ -2575,7 +2583,11 @@
           <t>[0-9]{5,}</t>
         </is>
       </c>
-      <c r="AU6" s="2" t="inlineStr"/>
+      <c r="AU6" s="2" t="inlineStr">
+        <is>
+          <t>[0-9]{4}-[0-9]{2}-[0-9]{2}</t>
+        </is>
+      </c>
       <c r="AV6" s="2" t="inlineStr"/>
       <c r="AW6" s="2" t="inlineStr"/>
       <c r="AX6" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@cb8b5855e785c054d8532791392a35340010100c 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="2037184015289833625" xfId="1" hidden="0"/>
-    <cellStyle name="6508422940602682099" xfId="2" hidden="0"/>
+    <cellStyle name="-6621635969532944098" xfId="1" hidden="0"/>
+    <cellStyle name="-9155632062852084468" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="AK2" s="2" t="inlineStr">
         <is>
-          <t>another description</t>
+          <t>Sequence of the I5 barcode</t>
         </is>
       </c>
       <c r="AL2" s="2" t="inlineStr">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="AK4" s="2" t="inlineStr">
         <is>
-          <t>Odomlab</t>
+          <t>Odomlab, ILSe</t>
         </is>
       </c>
       <c r="AL4" s="2" t="inlineStr">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="AM4" s="2" t="inlineStr">
         <is>
-          <t>Odomlab</t>
+          <t>Odomlab, ILSe</t>
         </is>
       </c>
       <c r="AN4" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@079109c57b77399740a7b75dabb01863b280eff9 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-4331516123719240021" xfId="1" hidden="0"/>
-    <cellStyle name="-9040223131899432966" xfId="2" hidden="0"/>
+    <cellStyle name="1507150893512826801" xfId="1" hidden="0"/>
+    <cellStyle name="-3843049994844073808" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@b672b8a1a03871ffc98a7132c117ce0baa3481ed 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-3181212514889753423" xfId="1" hidden="0"/>
-    <cellStyle name="-8304832868839875921" xfId="2" hidden="0"/>
+    <cellStyle name="-2002162457393507372" xfId="1" hidden="0"/>
+    <cellStyle name="-4492153878433722935" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@077b8b4415ab94e9e74b19455472edad0742c00f 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-2002162457393507372" xfId="1" hidden="0"/>
-    <cellStyle name="-4492153878433722935" xfId="2" hidden="0"/>
+    <cellStyle name="306505109779092096" xfId="1" hidden="0"/>
+    <cellStyle name="8412511059991164192" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="V4" s="2" t="inlineStr">
         <is>
-          <t>Odomlab, GUIDE</t>
+          <t>GUIDE, Odomlab</t>
         </is>
       </c>
       <c r="W4" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@22e186fa04dafd62e305c98ff82eb52ac42c0962 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="306505109779092096" xfId="1" hidden="0"/>
-    <cellStyle name="8412511059991164192" xfId="2" hidden="0"/>
+    <cellStyle name="-7306501240914249623" xfId="1" hidden="0"/>
+    <cellStyle name="6513355154185750121" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -480,10 +480,238 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="21" max="21"/>
+    <col width="20" customWidth="1" min="22" max="22"/>
+    <col width="20" customWidth="1" min="23" max="23"/>
+    <col width="20" customWidth="1" min="24" max="24"/>
+    <col width="20" customWidth="1" min="25" max="25"/>
+    <col width="20" customWidth="1" min="26" max="26"/>
+    <col width="20" customWidth="1" min="27" max="27"/>
+    <col width="20" customWidth="1" min="28" max="28"/>
+    <col width="20" customWidth="1" min="29" max="29"/>
+    <col width="20" customWidth="1" min="30" max="30"/>
+    <col width="20" customWidth="1" min="31" max="31"/>
+    <col width="20" customWidth="1" min="32" max="32"/>
+    <col width="20" customWidth="1" min="33" max="33"/>
+    <col width="20" customWidth="1" min="34" max="34"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SAMPLE_NAME_GPCF</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PROJECT</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PATIENT_ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SPECIES</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>STRAIN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>GENOME</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>INDIVIDUAL</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>SAMPLE_TYPE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>TISSUE</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>GENOTYPE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>PHENOTYPE</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SEX</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>DATE_OF_BIRTH</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>DATE_OF_DEATH</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>WAY_OF_DEATH</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>TREATMENT</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>CELL_INPUT[TOTAL_ALIVE CELLS]</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>TISSUE_PREP_METHOD</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>NA_PREP_METHOD</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>NOTES</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>LIB_PREP_KIT</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>AVERAGE_FRAGMENT_SIZE</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>BARCODETYPE</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>BARCODE_WELL_I5</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>BARCODE_SEQ_I5</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>BARCODE_WELL_I7</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>BARCODE_SEQ_I7</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>DNA_FRAGMENTATION_METHOD</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>IMAGING_DATASET_ID</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>MULTIPLEX_NAME</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>ILSE_NO</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>SINGLE_CELL_WELL_LABEL</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>ANTIBODY_TARGET</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>ANTIBODY</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AI6"/>
+  <sheetViews>
+    <sheetView rightToLeft="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -528,417 +756,177 @@
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>SAMPLE_NAME_GPCF</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>PROJECT</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>PATIENT_ID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>SPECIES</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>STRAIN</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>GENOME</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>INDIVIDUAL</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>SAMPLE_TYPE</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>TISSUE</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>GENOTYPE</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>PHENOTYPE</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>SEX</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>DATE_OF_BIRTH</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>DATE_OF_DEATH</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>WAY_OF_DEATH</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>TREATMENT</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>CELL_INPUT[TOTAL_ALIVE CELLS]</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>TISSUE_PREP_METHOD</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>NA_PREP_METHOD</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>NOTES</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>LIB_PREP_KIT</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>AVERAGE_FRAGMENT_SIZE</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>BARCODETYPE</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_WELL_I5</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_SEQ_I5</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_WELL_I7</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>BARCODE_SEQ_I7</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>DNA_FRAGMENTATION_METHOD</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>IMAGING_DATASET_ID</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>MULTIPLEX_NAME</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>ILSE_NO</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>SINGLE_CELL_WELL_LABEL</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY_TARGET</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>ANTIBODY</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>ANTIBODY_LOT</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AJ6"/>
-  <sheetViews>
-    <sheetView rightToLeft="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="20" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
-    <col width="20" customWidth="1" min="21" max="21"/>
-    <col width="20" customWidth="1" min="22" max="22"/>
-    <col width="20" customWidth="1" min="23" max="23"/>
-    <col width="20" customWidth="1" min="24" max="24"/>
-    <col width="20" customWidth="1" min="25" max="25"/>
-    <col width="20" customWidth="1" min="26" max="26"/>
-    <col width="20" customWidth="1" min="27" max="27"/>
-    <col width="20" customWidth="1" min="28" max="28"/>
-    <col width="20" customWidth="1" min="29" max="29"/>
-    <col width="20" customWidth="1" min="30" max="30"/>
-    <col width="20" customWidth="1" min="31" max="31"/>
-    <col width="20" customWidth="1" min="32" max="32"/>
-    <col width="20" customWidth="1" min="33" max="33"/>
-    <col width="20" customWidth="1" min="34" max="34"/>
-    <col width="20" customWidth="1" min="35" max="35"/>
-    <col width="20" customWidth="1" min="36" max="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>info</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>SAMPLE_NAME_GPCF</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PROJECT</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PATIENT_ID</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SPECIES</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>STRAIN</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>GENOME</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>INDIVIDUAL</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>SAMPLE_TYPE</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>TISSUE</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>GENOTYPE</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>PHENOTYPE</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>SEX</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>DATE_OF_BIRTH</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>DATE_OF_DEATH</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>WAY_OF_DEATH</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>TREATMENT</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>CELL_INPUT[TOTAL_ALIVE CELLS]</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>TISSUE_PREP_METHOD</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>NA_PREP_METHOD</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>NOTES</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>LIB_PREP_KIT</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>AVERAGE_FRAGMENT_SIZE</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>BARCODETYPE</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>BARCODE_WELL_I5</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>BARCODE_SEQ_I5</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>BARCODE_WELL_I7</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>BARCODE_SEQ_I7</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>DNA_FRAGMENTATION_METHOD</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>IMAGING_DATASET_ID</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>MULTIPLEX_NAME</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>ILSE_NO</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>SINGLE_CELL_WELL_LABEL</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>ANTIBODY_TARGET</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>ANTIBODY</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>ANTIBODY_LOT</t>
         </is>
       </c>
     </row>
@@ -1118,11 +1106,6 @@
           <t>Antibody name, manufacturer etc.</t>
         </is>
       </c>
-      <c r="AJ2" s="2" t="inlineStr">
-        <is>
-          <t>LOT number of the antibody</t>
-        </is>
-      </c>
     </row>
     <row r="3" ht="25" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
@@ -1282,7 +1265,6 @@
         </is>
       </c>
       <c r="AI3" s="2" t="inlineStr"/>
-      <c r="AJ3" s="2" t="inlineStr"/>
     </row>
     <row r="4" ht="25" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -1460,11 +1442,6 @@
           <t>Odomlab</t>
         </is>
       </c>
-      <c r="AJ4" s="2" t="inlineStr">
-        <is>
-          <t>Odomlab</t>
-        </is>
-      </c>
     </row>
     <row r="5" ht="25" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
@@ -1638,11 +1615,6 @@
         </is>
       </c>
       <c r="AI5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="AJ5" s="2" t="inlineStr">
         <is>
           <t>other</t>
         </is>
@@ -1740,7 +1712,6 @@
       </c>
       <c r="AH6" s="2" t="inlineStr"/>
       <c r="AI6" s="2" t="inlineStr"/>
-      <c r="AJ6" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@57a3f96a2cf8fbb891886b497c9a98d7b1974732 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-7306501240914249623" xfId="1" hidden="0"/>
-    <cellStyle name="6513355154185750121" xfId="2" hidden="0"/>
+    <cellStyle name="3894514756400538817" xfId="1" hidden="0"/>
+    <cellStyle name="-8348140008095211797" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@8ebed5f7bc0bd30ce46ccc40c9d55e1cea269fda 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-974054379579180369" xfId="1" hidden="0"/>
-    <cellStyle name="7230375233357039471" xfId="2" hidden="0"/>
+    <cellStyle name="7635079806406171085" xfId="1" hidden="0"/>
+    <cellStyle name="1108821744843284211" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -973,7 +973,7 @@
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Sample Type used by OTP, describing samples *across* individual, please follow guidelines</t>
+          <t>Sample Type used by OTP, describing samples *across* individual. (lowercase and dash(-) only, end with digit)</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
@@ -1649,7 +1649,11 @@
       <c r="F6" s="2" t="inlineStr"/>
       <c r="G6" s="2" t="inlineStr"/>
       <c r="H6" s="2" t="inlineStr"/>
-      <c r="I6" s="2" t="inlineStr"/>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>[a-z0-9-]*</t>
+        </is>
+      </c>
       <c r="J6" s="2" t="inlineStr"/>
       <c r="K6" s="2" t="inlineStr"/>
       <c r="L6" s="2" t="inlineStr"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@84bb15fadd74858077f6f693109ae49e7b22d7fa 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="7635079806406171085" xfId="1" hidden="0"/>
-    <cellStyle name="1108821744843284211" xfId="2" hidden="0"/>
+    <cellStyle name="7974266402926894508" xfId="1" hidden="0"/>
+    <cellStyle name="2685469106096664587" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@34c5c14b6b669ee4e6b2ab8b1ebfc5017d763a69 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="2756097199724357391" xfId="1" hidden="0"/>
-    <cellStyle name="-731146629961624635" xfId="2" hidden="0"/>
+    <cellStyle name="2580808146492040243" xfId="1" hidden="0"/>
+    <cellStyle name="7079948450441415062" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AB2" s="2" t="inlineStr">
         <is>
-          <t>Sequence of the I7 barcode (for 10x-singcell this can be a comma-separated list of 4 indeces)</t>
+          <t>Sequence of the I7 barcode (for 10x-Single Cell, you need enter four rows to supply the barcodes and add a "_a,_b,_c, _d" suffix to the Sample Type)</t>
         </is>
       </c>
       <c r="AC2" s="2" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="AB3" s="2" t="inlineStr">
         <is>
-          <t>TTACCGAC, GCGAGTAA</t>
+          <t>TTACCGAC</t>
         </is>
       </c>
       <c r="AC3" s="2" t="inlineStr">
@@ -1694,7 +1694,7 @@
       <c r="AA6" s="2" t="inlineStr"/>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>[ATGC, ]*</t>
+          <t>[ATGC]*</t>
         </is>
       </c>
       <c r="AC6" s="2" t="inlineStr"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@ecceaecc586c80efda8dfb9a7b0d0c786cd2a094 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.by_category.xlsx
+++ b/sheets/sequencing_spreadsheet_template.by_category.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-8636662239298810035" xfId="1" hidden="0"/>
-    <cellStyle name="-3644374285188671303" xfId="2" hidden="0"/>
+    <cellStyle name="4776989127365596862" xfId="1" hidden="0"/>
+    <cellStyle name="-4981025973110287276" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>